<commit_message>
Analysis as of Sept 2021 Submission
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8178,7 +8178,11 @@
           <t>psg</t>
         </is>
       </c>
-      <c r="S85" t="inlineStr"/>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>mild</t>
+        </is>
+      </c>
       <c r="T85" t="inlineStr">
         <is>
           <t>cpap</t>
@@ -11942,7 +11946,7 @@
       </c>
       <c r="S126" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T126" t="inlineStr">
@@ -15898,7 +15902,7 @@
       </c>
       <c r="S169" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T169" t="inlineStr">
@@ -16174,7 +16178,7 @@
       </c>
       <c r="S172" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T172" t="inlineStr">
@@ -18192,7 +18196,7 @@
       </c>
       <c r="S194" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T194" t="inlineStr">
@@ -18652,7 +18656,7 @@
       </c>
       <c r="S199" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T199" t="inlineStr">
@@ -19020,7 +19024,7 @@
       </c>
       <c r="S203" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T203" t="inlineStr">
@@ -19754,7 +19758,7 @@
       </c>
       <c r="S211" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T211" t="inlineStr">
@@ -21502,7 +21506,7 @@
       </c>
       <c r="S230" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T230" t="inlineStr">
@@ -21686,7 +21690,7 @@
       </c>
       <c r="S232" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T232" t="inlineStr">
@@ -45962,7 +45966,7 @@
       </c>
       <c r="S496" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>mild</t>
         </is>
       </c>
       <c r="T496" t="inlineStr">

</xml_diff>